<commit_message>
Made some changes to allow the Julia model to be called form the Spine Toolbox project.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59D0A8C-29C1-45BF-BB08-982C5F5C12C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F72F16-B700-4AC1-AACC-BC82BAA21B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="3375" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="commodities" sheetId="9" r:id="rId1"/>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,7 +700,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
@@ -964,7 +964,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L6"/>
+      <selection activeCell="C6" sqref="C6:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1238,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71A3C8B-32E4-43A2-86A7-9D0D83F1C332}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Made some changes to input data structure and content.
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,17 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F72F16-B700-4AC1-AACC-BC82BAA21B85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37DCFC2-4C4D-4D98-B9C2-80EC7BE8C0FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="3375" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="commodities" sheetId="9" r:id="rId1"/>
+    <sheet name="resources" sheetId="9" r:id="rId1"/>
     <sheet name="node_def" sheetId="1" r:id="rId2"/>
-    <sheet name="unit_def" sheetId="2" r:id="rId3"/>
+    <sheet name="process_def" sheetId="2" r:id="rId3"/>
     <sheet name="flow" sheetId="5" r:id="rId4"/>
     <sheet name="prices" sheetId="6" r:id="rId5"/>
-    <sheet name="transfer" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,10 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
-  <si>
-    <t>commodity</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>dh</t>
   </si>
@@ -52,9 +48,6 @@
     <t>wind</t>
   </si>
   <si>
-    <t>balance</t>
-  </si>
-  <si>
     <t>gas</t>
   </si>
   <si>
@@ -64,9 +57,6 @@
     <t>bio</t>
   </si>
   <si>
-    <t>unit</t>
-  </si>
-  <si>
     <t>eff</t>
   </si>
   <si>
@@ -88,24 +78,6 @@
     <t>unit_bio1</t>
   </si>
   <si>
-    <t>node_from</t>
-  </si>
-  <si>
-    <t>node_to</t>
-  </si>
-  <si>
-    <t>cap_from</t>
-  </si>
-  <si>
-    <t>cap_to</t>
-  </si>
-  <si>
-    <t>losses</t>
-  </si>
-  <si>
-    <t>0.01</t>
-  </si>
-  <si>
     <t>input_node</t>
   </si>
   <si>
@@ -124,15 +96,6 @@
     <t>unit_gt2</t>
   </si>
   <si>
-    <t>transfer</t>
-  </si>
-  <si>
-    <t>node_dh1__to__node_dh2</t>
-  </si>
-  <si>
-    <t>node_elec1__to__node_elec2</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -160,9 +123,6 @@
     <t>VOM_cost</t>
   </si>
   <si>
-    <t>0.5</t>
-  </si>
-  <si>
     <t>min_load</t>
   </si>
   <si>
@@ -184,10 +144,46 @@
     <t>unit_windturb1</t>
   </si>
   <si>
-    <t>wind_availableB</t>
-  </si>
-  <si>
     <t>windB</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>is_commodity</t>
+  </si>
+  <si>
+    <t>has_balance</t>
+  </si>
+  <si>
+    <t>process</t>
+  </si>
+  <si>
+    <t>transfer_dhA_dhB</t>
+  </si>
+  <si>
+    <t>transfer_dhB_dhB</t>
+  </si>
+  <si>
+    <t>transfer_elecA_elecB</t>
+  </si>
+  <si>
+    <t>transfer_elecB_elecA</t>
+  </si>
+  <si>
+    <t>ramp_up</t>
+  </si>
+  <si>
+    <t>ramp_down</t>
+  </si>
+  <si>
+    <t>online</t>
+  </si>
+  <si>
+    <t>unit_CHP1_dh</t>
+  </si>
+  <si>
+    <t>unit_CHP1_elec</t>
   </si>
 </sst>
 </file>
@@ -515,47 +511,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF99E4D-86B0-48F4-832E-8948932567B4}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+      <c r="B7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -565,10 +582,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,21 +596,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -602,10 +619,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -614,10 +631,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -626,10 +643,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -637,10 +654,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -648,10 +665,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -659,10 +676,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -670,24 +687,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -697,261 +703,553 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B317E83-B82C-4F97-9016-F4FF07D7D9BF}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>0.2</v>
+      </c>
+      <c r="L2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <v>0.1</v>
+      </c>
+      <c r="L3">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4">
+        <v>0.2</v>
+      </c>
+      <c r="L4">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0.4</v>
+      </c>
+      <c r="L5">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>41</v>
-      </c>
-      <c r="H1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0.2</v>
+      </c>
+      <c r="L7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>5</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5">
-        <v>5</v>
-      </c>
-      <c r="E5">
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
         <v>2</v>
       </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6">
-        <v>4</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8">
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
         <v>7</v>
       </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>0.1</v>
+      </c>
+      <c r="L8">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>47</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0.4</v>
+      </c>
+      <c r="H9">
+        <v>0.3</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1"/>
+      <c r="K9">
+        <v>0.3</v>
+      </c>
+      <c r="L9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0.4</v>
+      </c>
+      <c r="H10">
+        <v>0.3</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="K10">
+        <v>0.1</v>
+      </c>
+      <c r="L10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
-        <v>5</v>
-      </c>
-      <c r="E9" t="s">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11">
+        <v>0.2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11">
+        <v>0.3</v>
+      </c>
+      <c r="L11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>48</v>
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0.99</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>0.5</v>
+      </c>
+      <c r="L12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0.99</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0.4</v>
+      </c>
+      <c r="L13">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.99</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <v>0.4</v>
+      </c>
+      <c r="L14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0.99</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <v>0.5</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>
@@ -961,140 +1259,133 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD40D804-01EB-47A4-AE91-C7D0229E2D4B}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:L6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="4">
+        <v>43831</v>
+      </c>
       <c r="C1" s="4">
-        <v>43831</v>
+        <v>43832</v>
       </c>
       <c r="D1" s="4">
-        <v>43832</v>
+        <v>43833</v>
       </c>
       <c r="E1" s="4">
-        <v>43833</v>
+        <v>43834</v>
       </c>
       <c r="F1" s="4">
-        <v>43834</v>
+        <v>43835</v>
       </c>
       <c r="G1" s="4">
-        <v>43835</v>
+        <v>43836</v>
       </c>
       <c r="H1" s="4">
-        <v>43836</v>
+        <v>43837</v>
       </c>
       <c r="I1" s="4">
-        <v>43837</v>
+        <v>43838</v>
       </c>
       <c r="J1" s="4">
-        <v>43838</v>
+        <v>43839</v>
       </c>
       <c r="K1" s="4">
-        <v>43839</v>
-      </c>
-      <c r="L1" s="4">
         <v>43840</v>
       </c>
+      <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>32</v>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="3">
+        <v>-1.8</v>
       </c>
       <c r="C2" s="3">
-        <v>-1.8</v>
+        <v>-3.5</v>
       </c>
       <c r="D2" s="3">
+        <v>-6.6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>-12.7</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-12.8</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-10</v>
+      </c>
+      <c r="H2" s="3">
+        <v>-7.7</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-7.6</v>
+      </c>
+      <c r="J2" s="3">
+        <v>-2.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>-3.7</v>
+      </c>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="3">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-3.6</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-4.2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-7.1</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-11.1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>-6.4</v>
+      </c>
+      <c r="H3" s="3">
+        <v>-3.3</v>
+      </c>
+      <c r="I3" s="3">
         <v>-3.5</v>
       </c>
-      <c r="E2" s="3">
-        <v>-6.6</v>
-      </c>
-      <c r="F2" s="3">
-        <v>-12.7</v>
-      </c>
-      <c r="G2" s="3">
-        <v>-12.8</v>
-      </c>
-      <c r="H2" s="3">
-        <v>-10</v>
-      </c>
-      <c r="I2" s="3">
-        <v>-7.7</v>
-      </c>
-      <c r="J2" s="3">
-        <v>-7.6</v>
-      </c>
-      <c r="K2" s="3">
-        <v>-2.5</v>
-      </c>
-      <c r="L2" s="3">
-        <v>-3.7</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="D3" s="3">
-        <v>-3.6</v>
-      </c>
-      <c r="E3" s="3">
-        <v>-4.2</v>
-      </c>
-      <c r="F3" s="3">
-        <v>-7.1</v>
-      </c>
-      <c r="G3" s="3">
-        <v>-11.1</v>
-      </c>
-      <c r="H3" s="3">
-        <v>-6.4</v>
-      </c>
-      <c r="I3" s="3">
-        <v>-3.3</v>
-      </c>
       <c r="J3" s="3">
-        <v>-3.5</v>
+        <v>-2.1</v>
       </c>
       <c r="K3" s="3">
-        <v>-2.1</v>
-      </c>
-      <c r="L3" s="3">
         <v>-2.2000000000000002</v>
       </c>
+      <c r="M3" s="3"/>
       <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-    </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-2</v>
       </c>
       <c r="C4" s="3">
         <v>-2</v>
@@ -1123,94 +1414,86 @@
       <c r="K4" s="3">
         <v>-2</v>
       </c>
-      <c r="L4" s="3">
-        <v>-2</v>
-      </c>
+      <c r="M4" s="3"/>
       <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-    </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3">
+        <v>-1.1000000000000001</v>
       </c>
       <c r="C5" s="3">
+        <v>-1.2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-0.9</v>
+      </c>
+      <c r="E5" s="3">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="D5" s="3">
+      <c r="F5" s="3">
+        <v>-0.8</v>
+      </c>
+      <c r="G5" s="3">
         <v>-1.2</v>
-      </c>
-      <c r="E5" s="3">
-        <v>-0.9</v>
-      </c>
-      <c r="F5" s="3">
-        <v>-1.1000000000000001</v>
-      </c>
-      <c r="G5" s="3">
-        <v>-0.8</v>
       </c>
       <c r="H5" s="3">
         <v>-1.2</v>
       </c>
       <c r="I5" s="3">
+        <v>-1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>-0.8</v>
+      </c>
+      <c r="K5" s="3">
         <v>-1.2</v>
       </c>
-      <c r="J5" s="3">
-        <v>-1</v>
-      </c>
-      <c r="K5" s="3">
-        <v>-0.8</v>
-      </c>
-      <c r="L5" s="3">
-        <v>-1.2</v>
-      </c>
+      <c r="M5" s="3"/>
       <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-    </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.2999999999999998</v>
       </c>
       <c r="C6" s="3">
-        <v>4.5</v>
+        <v>1.6</v>
       </c>
       <c r="D6" s="3">
-        <v>3.1</v>
+        <v>2.1</v>
       </c>
       <c r="E6" s="3">
-        <v>3.6</v>
+        <v>1.4</v>
       </c>
       <c r="F6" s="3">
-        <v>3.1</v>
+        <v>1.7</v>
       </c>
       <c r="G6" s="3">
-        <v>3.4</v>
+        <v>1.3</v>
       </c>
       <c r="H6" s="3">
-        <v>3.9</v>
+        <v>0.7</v>
       </c>
       <c r="I6" s="3">
-        <v>4.8</v>
+        <v>0.6</v>
       </c>
       <c r="J6" s="3">
-        <v>4.8</v>
+        <v>0.7</v>
       </c>
       <c r="K6" s="3">
-        <v>4.2</v>
-      </c>
-      <c r="L6" s="3">
-        <v>3.9</v>
-      </c>
+        <v>0.7</v>
+      </c>
+      <c r="M6" s="3"/>
       <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-    </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7"/>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7"/>
+      <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -1220,12 +1503,11 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1238,7 +1520,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71A3C8B-32E4-43A2-86A7-9D0D83F1C332}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1276,7 +1560,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1311,7 +1595,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -1346,7 +1630,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>8</v>
@@ -1381,7 +1665,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1416,7 +1700,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>10</v>
@@ -1451,7 +1735,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1488,96 +1772,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCF7DCD5-37F1-4A06-946A-7D41EC709552}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Changed input data excel and importer mapping to function better as a demo case
</commit_message>
<xml_diff>
--- a/input_data/input_data.xlsx
+++ b/input_data/input_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsdennis\HOPE\Predicer\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37DCFC2-4C4D-4D98-B9C2-80EC7BE8C0FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FBCA8BA-398E-40A8-A677-1B154A4F0629}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5115" yWindow="3045" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="resources" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>dh</t>
   </si>
@@ -184,6 +184,12 @@
   </si>
   <si>
     <t>unit_CHP1_elec</t>
+  </si>
+  <si>
+    <t>is_CF</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -584,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +610,9 @@
       <c r="C1" t="s">
         <v>38</v>
       </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -615,6 +624,9 @@
       <c r="C2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,7 +639,9 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -639,7 +653,9 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -650,6 +666,9 @@
       </c>
       <c r="C5">
         <v>1</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -662,6 +681,9 @@
       <c r="C6">
         <v>0</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -673,6 +695,9 @@
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -684,6 +709,9 @@
       <c r="C8">
         <v>0</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -693,6 +721,9 @@
         <v>35</v>
       </c>
       <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
         <v>1</v>
       </c>
     </row>
@@ -705,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B317E83-B82C-4F97-9016-F4FF07D7D9BF}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,8 +1551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A71A3C8B-32E4-43A2-86A7-9D0D83F1C332}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>